<commit_message>
made working for level 5, 2nd sem
</commit_message>
<xml_diff>
--- a/individual_routines/L5CG10_routine_3rdSem.xlsx
+++ b/individual_routines/L5CG10_routine_3rdSem.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -459,17 +459,27 @@
       </c>
       <c r="H1" t="inlineStr">
         <is>
+          <t>Room</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>Block</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
           <t>Group</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>Block</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>Room</t>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>Level</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>Course</t>
         </is>
       </c>
     </row>
@@ -481,85 +491,93 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>11:00-13:30</t>
+          <t>7:00-9:00</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>5CS019</t>
+          <t>5CS022</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Object-Oriented Design and Programming</t>
+          <t>Human Computer Interaction</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Workshop</t>
+          <t>Tutorial</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Mr. Bishal Khadka</t>
+          <t>Mr. Apurba Neupane</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
+          <t>SR-03 Wolves</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>WLV</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
           <t>L5CG10</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>HCK</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>Lab04-Patan</t>
+      <c r="K2" t="n">
+        <v>5</v>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>BCS</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>MON</t>
+          <t>SUN</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>9:00-11:00</t>
+          <t>9:30-12:00</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>5CS021</t>
+          <t>5CS024</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Numerical Methods and Concurrency</t>
+          <t>Collaborative Development</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Lecture</t>
+          <t>Workshop</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Mr. Udaya Kandel</t>
+          <t>Mr. Anmol Adhikari</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>L5CG10+L5CG11</t>
+          <t>SR-03 Wolves</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -569,7 +587,15 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>LT03-Lecture Theater 03</t>
+          <t>L5CG10</t>
+        </is>
+      </c>
+      <c r="K3" t="n">
+        <v>5</v>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>BCS</t>
         </is>
       </c>
     </row>
@@ -581,17 +607,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>12:00-14:30</t>
+          <t>7:00-9:30</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>5CS037</t>
+          <t>5CS022</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Concepts and Technologies of AI</t>
+          <t>Human Computer Interaction</t>
         </is>
       </c>
       <c r="E4" t="n">
@@ -604,22 +630,30 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Mr. Anmol Adhikari</t>
+          <t>Mr. Apurba Neupane</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
+          <t>Lab-03 Gahanapokhari</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>HCK</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
           <t>L5CG10</t>
         </is>
       </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>HCK</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>SR02-Seminar Room 02</t>
+      <c r="K4" t="n">
+        <v>5</v>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>BCS</t>
         </is>
       </c>
     </row>
@@ -631,17 +665,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>7:00-9:00</t>
+          <t>9:30-11:30</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>5CS019</t>
+          <t>5CS024</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Object-Oriented Design and Programming</t>
+          <t>Collaborative Development</t>
         </is>
       </c>
       <c r="E5" t="n">
@@ -654,12 +688,12 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Mr. Deepson Shrestha</t>
+          <t>Mr. Udaya Kandel</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>L5CG10+L5CG11</t>
+          <t>LT-03 Walsall</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
@@ -669,7 +703,15 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>LT01-Lecture Theater 01</t>
+          <t>L5CG(9+10+11)</t>
+        </is>
+      </c>
+      <c r="K5" t="n">
+        <v>5</v>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>BCS</t>
         </is>
       </c>
     </row>
@@ -681,17 +723,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>10:00-12:00</t>
+          <t>12:00-14:00</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>5CS037</t>
+          <t>5CS022</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Concepts and Technologies of AI</t>
+          <t>Human Computer Interaction</t>
         </is>
       </c>
       <c r="E6" t="n">
@@ -704,12 +746,12 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Mr. Prakash Gautam</t>
+          <t>Mr. Pravash Karki</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>L5CG8+L5CG9+L5CG10+L5CG11</t>
+          <t>LT-02 Telford</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
@@ -719,7 +761,15 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>LT02-Lecture Theater 02</t>
+          <t>L5CG(9+10+11)</t>
+        </is>
+      </c>
+      <c r="K6" t="n">
+        <v>5</v>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>BCS</t>
         </is>
       </c>
     </row>
@@ -736,12 +786,12 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>5CS021</t>
+          <t>5CS020</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Numerical Methods and Concurrency</t>
+          <t>Distributed and Cloud Systems Programming</t>
         </is>
       </c>
       <c r="E7" t="n">
@@ -749,17 +799,17 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Tutorial</t>
+          <t>Lecture</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Mr. Udaya Kandel</t>
+          <t>Mr. Sumanta Silwal</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>L5CG10</t>
+          <t>LT-02 Telford</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
@@ -769,57 +819,73 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>SR03-Seminar Room 03</t>
+          <t>L5CG(9+10+11)</t>
+        </is>
+      </c>
+      <c r="K7" t="n">
+        <v>5</v>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>BCS</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>THU</t>
+          <t>WED</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>9:00-11:30</t>
+          <t>12:30-14:30</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>5CS021</t>
+          <t>5CS024</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Numerical Methods and Concurrency</t>
+          <t>Collaborative Development</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Workshop</t>
+          <t>Tutorial</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Mr. Udaya Kandel</t>
+          <t>Mr. Anmol Adhikari</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
+          <t>TR-09  Chandragiri</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>HCK</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
           <t>L5CG10</t>
         </is>
       </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>WLV</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>SR04-Seminar Room 04</t>
+      <c r="K8" t="n">
+        <v>5</v>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>BCS</t>
         </is>
       </c>
     </row>
@@ -836,12 +902,12 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>5CS037</t>
+          <t>5CS020</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Concepts and Technologies of AI</t>
+          <t>Distributed and Cloud Systems Programming</t>
         </is>
       </c>
       <c r="E9" t="n">
@@ -854,22 +920,30 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Mr. Anmol Adhikari</t>
+          <t>Mr. Deepson Shrestha</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
+          <t>SR-01 Bantok</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>WLV</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
           <t>L5CG10</t>
         </is>
       </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>WLV</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>SR04-Seminar Room 04</t>
+      <c r="K9" t="n">
+        <v>5</v>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>BCS</t>
         </is>
       </c>
     </row>
@@ -881,45 +955,53 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>7:00-9:00</t>
+          <t>9:30-12:00</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>5CS019</t>
+          <t>5CS020</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Object-Oriented Design and Programming</t>
+          <t>Distributed and Cloud Systems Programming</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Tutorial</t>
+          <t>Workshop</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Mr. Bishal Khadka</t>
+          <t>Mr. Deepson Shrestha</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
+          <t>Lab-02 Moseley</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>WLV</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
           <t>L5CG10</t>
         </is>
       </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>HCK</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>TR05-Ranipokhari</t>
+      <c r="K10" t="n">
+        <v>5</v>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>BCS</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
updated for new routine
</commit_message>
<xml_diff>
--- a/individual_routines/L5CG10_routine_3rdSem.xlsx
+++ b/individual_routines/L5CG10_routine_3rdSem.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,62 +424,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Day</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Time</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Module Code</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Module Title</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>Hours</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>Class Type</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>Lecturer</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>Room</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>Block</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>Group</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>Level</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>Course</t>
+          <t>Herald College Kathmandu</t>
         </is>
       </c>
     </row>
@@ -494,19 +439,19 @@
           <t>7:00-9:00</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D2" t="inlineStr">
         <is>
           <t>5CS022</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t>Human Computer Interaction</t>
         </is>
       </c>
-      <c r="E2" t="n">
-        <v>2</v>
-      </c>
       <c r="F2" t="inlineStr">
         <is>
           <t>Tutorial</t>
@@ -519,25 +464,17 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
+          <t>L5CG10</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>WLV</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
           <t>SR-03 Wolves</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>WLV</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>L5CG10</t>
-        </is>
-      </c>
-      <c r="K2" t="n">
-        <v>5</v>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>BCS</t>
         </is>
       </c>
     </row>
@@ -552,19 +489,19 @@
           <t>9:30-12:00</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="C3" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="D3" t="inlineStr">
         <is>
           <t>5CS024</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="E3" t="inlineStr">
         <is>
           <t>Collaborative Development</t>
         </is>
       </c>
-      <c r="E3" t="n">
-        <v>2.5</v>
-      </c>
       <c r="F3" t="inlineStr">
         <is>
           <t>Workshop</t>
@@ -577,25 +514,17 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
+          <t>L5CG10</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>WLV</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
           <t>SR-03 Wolves</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>WLV</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>L5CG10</t>
-        </is>
-      </c>
-      <c r="K3" t="n">
-        <v>5</v>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>BCS</t>
         </is>
       </c>
     </row>
@@ -610,19 +539,19 @@
           <t>7:00-9:30</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="C4" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="D4" t="inlineStr">
         <is>
           <t>5CS022</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="E4" t="inlineStr">
         <is>
           <t>Human Computer Interaction</t>
         </is>
       </c>
-      <c r="E4" t="n">
-        <v>2.5</v>
-      </c>
       <c r="F4" t="inlineStr">
         <is>
           <t>Workshop</t>
@@ -635,25 +564,17 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
+          <t>L5CG10</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>HCK</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
           <t>Lab-03 Gahanapokhari</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>HCK</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>L5CG10</t>
-        </is>
-      </c>
-      <c r="K4" t="n">
-        <v>5</v>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>BCS</t>
         </is>
       </c>
     </row>
@@ -668,19 +589,19 @@
           <t>9:30-11:30</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="C5" t="n">
+        <v>2</v>
+      </c>
+      <c r="D5" t="inlineStr">
         <is>
           <t>5CS024</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="E5" t="inlineStr">
         <is>
           <t>Collaborative Development</t>
         </is>
       </c>
-      <c r="E5" t="n">
-        <v>2</v>
-      </c>
       <c r="F5" t="inlineStr">
         <is>
           <t>Lecture</t>
@@ -693,25 +614,17 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
+          <t>L5CG(9+10+11)</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>WLV</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
           <t>LT-03 Walsall</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>WLV</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>L5CG(9+10+11)</t>
-        </is>
-      </c>
-      <c r="K5" t="n">
-        <v>5</v>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>BCS</t>
         </is>
       </c>
     </row>
@@ -726,19 +639,19 @@
           <t>12:00-14:00</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="C6" t="n">
+        <v>2</v>
+      </c>
+      <c r="D6" t="inlineStr">
         <is>
           <t>5CS022</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="E6" t="inlineStr">
         <is>
           <t>Human Computer Interaction</t>
         </is>
       </c>
-      <c r="E6" t="n">
-        <v>2</v>
-      </c>
       <c r="F6" t="inlineStr">
         <is>
           <t>Lecture</t>
@@ -751,25 +664,17 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
+          <t>L5CG(9+10+11)</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>WLV</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
           <t>LT-02 Telford</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>WLV</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>L5CG(9+10+11)</t>
-        </is>
-      </c>
-      <c r="K6" t="n">
-        <v>5</v>
-      </c>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t>BCS</t>
         </is>
       </c>
     </row>
@@ -784,19 +689,19 @@
           <t>9:00-11:00</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="C7" t="n">
+        <v>2</v>
+      </c>
+      <c r="D7" t="inlineStr">
         <is>
           <t>5CS020</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="E7" t="inlineStr">
         <is>
           <t>Distributed and Cloud Systems Programming</t>
         </is>
       </c>
-      <c r="E7" t="n">
-        <v>2</v>
-      </c>
       <c r="F7" t="inlineStr">
         <is>
           <t>Lecture</t>
@@ -809,25 +714,17 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
+          <t>L5CG(9+10+11)</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>WLV</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
           <t>LT-02 Telford</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>WLV</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>L5CG(9+10+11)</t>
-        </is>
-      </c>
-      <c r="K7" t="n">
-        <v>5</v>
-      </c>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t>BCS</t>
         </is>
       </c>
     </row>
@@ -842,19 +739,19 @@
           <t>12:30-14:30</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="C8" t="n">
+        <v>2</v>
+      </c>
+      <c r="D8" t="inlineStr">
         <is>
           <t>5CS024</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="E8" t="inlineStr">
         <is>
           <t>Collaborative Development</t>
         </is>
       </c>
-      <c r="E8" t="n">
-        <v>2</v>
-      </c>
       <c r="F8" t="inlineStr">
         <is>
           <t>Tutorial</t>
@@ -867,25 +764,17 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
+          <t>L5CG10</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>HCK</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
           <t>TR-09  Chandragiri</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>HCK</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>L5CG10</t>
-        </is>
-      </c>
-      <c r="K8" t="n">
-        <v>5</v>
-      </c>
-      <c r="L8" t="inlineStr">
-        <is>
-          <t>BCS</t>
         </is>
       </c>
     </row>
@@ -900,19 +789,19 @@
           <t>13:00-15:00</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="C9" t="n">
+        <v>2</v>
+      </c>
+      <c r="D9" t="inlineStr">
         <is>
           <t>5CS020</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="E9" t="inlineStr">
         <is>
           <t>Distributed and Cloud Systems Programming</t>
         </is>
       </c>
-      <c r="E9" t="n">
-        <v>2</v>
-      </c>
       <c r="F9" t="inlineStr">
         <is>
           <t>Tutorial</t>
@@ -925,25 +814,17 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
+          <t>L5CG10</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>WLV</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
           <t>SR-01 Bantok</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>WLV</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>L5CG10</t>
-        </is>
-      </c>
-      <c r="K9" t="n">
-        <v>5</v>
-      </c>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>BCS</t>
         </is>
       </c>
     </row>
@@ -958,19 +839,19 @@
           <t>9:30-12:00</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="C10" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="D10" t="inlineStr">
         <is>
           <t>5CS020</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
+      <c r="E10" t="inlineStr">
         <is>
           <t>Distributed and Cloud Systems Programming</t>
         </is>
       </c>
-      <c r="E10" t="n">
-        <v>2.5</v>
-      </c>
       <c r="F10" t="inlineStr">
         <is>
           <t>Workshop</t>
@@ -983,25 +864,17 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
+          <t>L5CG10</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>WLV</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
           <t>Lab-02 Moseley</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>WLV</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>L5CG10</t>
-        </is>
-      </c>
-      <c r="K10" t="n">
-        <v>5</v>
-      </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>BCS</t>
         </is>
       </c>
     </row>

</xml_diff>